<commit_message>
Added 2 more lines to the step_template_e, tried to do the same as temperatures
</commit_message>
<xml_diff>
--- a/part_2/files/lateral/surface_behav.xlsx
+++ b/part_2/files/lateral/surface_behav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\new\madina_abaqus\lateral\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\madina_abaqus\part_2\files\lateral\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE0F010-DBFA-4BD3-8F00-4EEAE8570B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A86A05-0430-46B8-8814-78A4647AD560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,10 +352,13 @@
   <dimension ref="A1:C1220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">

</xml_diff>